<commit_message>
Update with Dr. Oh
</commit_message>
<xml_diff>
--- a/polls/ICRA2020Workshops.xlsx
+++ b/polls/ICRA2020Workshops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6E7B7A-AD5C-49CA-AA78-697762A1C6EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9537563C-5A5A-43D6-BD39-6E1FAF50EFE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,9 +639,6 @@
     <t>Robot Accident Investigation: a case study in Responsible Robotics</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=mjGW52_BvPc&amp;feature=youtu.be</t>
-  </si>
-  <si>
     <t>Dag Balkmar</t>
   </si>
   <si>
@@ -841,6 +838,9 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1hrYXzCPe_V8FplsBDMaamCOMuf4QZXbF/preview</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/mjGW52_BvPc</t>
   </si>
 </sst>
 </file>
@@ -1237,20 +1237,20 @@
   <dimension ref="A1:BJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1283,7 +1283,7 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M1" t="s">
         <v>33</v>
@@ -1400,43 +1400,43 @@
         <v>142</v>
       </c>
       <c r="AY1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>246</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>247</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>248</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>249</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>250</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>251</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>252</v>
       </c>
-      <c r="BF1" t="s">
-        <v>253</v>
-      </c>
       <c r="BG1" t="s">
+        <v>260</v>
+      </c>
+      <c r="BH1" t="s">
         <v>261</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>262</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>263</v>
       </c>
-      <c r="BJ1" t="s">
-        <v>264</v>
-      </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="AD2" s="1"/>
       <c r="AH2" s="1"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1497,12 +1497,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1613,7 +1613,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>99</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K9" t="s">
         <v>100</v>
@@ -1813,7 +1813,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2031,12 +2031,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" t="s">
         <v>200</v>
@@ -2057,166 +2057,166 @@
         <v>204</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="K15" t="s">
         <v>205</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>206</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>207</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" t="s">
         <v>209</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>210</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>211</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" t="s">
         <v>213</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>214</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>215</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="W15" t="s">
         <v>217</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>218</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>219</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="Z15" s="1" t="s">
+      <c r="AA15" t="s">
         <v>221</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AB15" t="s">
         <v>222</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>223</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AD15" s="1" t="s">
+      <c r="AE15" t="s">
         <v>225</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AF15" t="s">
         <v>226</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AG15" t="s">
         <v>227</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AH15" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="AH15" s="1" t="s">
+      <c r="AI15" t="s">
         <v>229</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AJ15" t="s">
         <v>230</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AK15" t="s">
         <v>231</v>
       </c>
-      <c r="AK15" t="s">
+      <c r="AL15" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="AL15" s="1" t="s">
+      <c r="AM15" t="s">
         <v>233</v>
       </c>
-      <c r="AM15" t="s">
+      <c r="AN15" t="s">
         <v>234</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AO15" t="s">
         <v>235</v>
       </c>
-      <c r="AO15" t="s">
+      <c r="AP15" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AP15" s="1" t="s">
+      <c r="AQ15" t="s">
         <v>237</v>
       </c>
-      <c r="AQ15" t="s">
+      <c r="AR15" t="s">
         <v>238</v>
       </c>
-      <c r="AR15" t="s">
+      <c r="AS15" t="s">
         <v>239</v>
       </c>
-      <c r="AS15" t="s">
+      <c r="AT15" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="AT15" s="1" t="s">
+      <c r="AU15" t="s">
         <v>241</v>
       </c>
-      <c r="AU15" t="s">
+      <c r="AV15" t="s">
         <v>242</v>
       </c>
-      <c r="AV15" t="s">
+      <c r="AW15" t="s">
         <v>243</v>
       </c>
-      <c r="AW15" t="s">
+      <c r="AX15" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="AX15" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="AY15" t="s">
+        <v>253</v>
+      </c>
+      <c r="AZ15" t="s">
         <v>254</v>
       </c>
-      <c r="AZ15" t="s">
+      <c r="BA15" t="s">
         <v>255</v>
       </c>
-      <c r="BA15" t="s">
+      <c r="BB15" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="BB15" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="BC15" t="s">
         <v>171</v>
       </c>
       <c r="BD15" t="s">
+        <v>257</v>
+      </c>
+      <c r="BE15" t="s">
         <v>258</v>
       </c>
-      <c r="BE15" t="s">
+      <c r="BF15" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="BF15" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="BG15" t="s">
         <v>79</v>
       </c>
       <c r="BH15" t="s">
+        <v>264</v>
+      </c>
+      <c r="BI15" t="s">
         <v>265</v>
       </c>
-      <c r="BI15" t="s">
+      <c r="BJ15" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="BJ15" s="1" t="s">
-        <v>267</v>
-      </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
     </row>
   </sheetData>
@@ -2260,23 +2260,24 @@
     <hyperlink ref="D13" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
     <hyperlink ref="D14" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
     <hyperlink ref="D15" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="J15" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="N15" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="R15" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="V15" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="Z15" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="AD15" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="AH15" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="AL15" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="AP15" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="AT15" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="AX15" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="BB15" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="BF15" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="BJ15" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="N15" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="R15" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="V15" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="Z15" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="AD15" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="AH15" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="AL15" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="AP15" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="AT15" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="AX15" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="BB15" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="BF15" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="BJ15" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="J9" r:id="rId53" xr:uid="{F6D4B88A-C6E6-4468-97F9-C526CEE91C2B}"/>
+    <hyperlink ref="J15" r:id="rId54" xr:uid="{C9E3645C-04D8-4200-BC9B-9B7ECA30CE64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId54"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId55"/>
 </worksheet>
 </file>
 
@@ -2286,7 +2287,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2298,7 +2299,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finally Comments are implemented
good job for both of us
</commit_message>
<xml_diff>
--- a/polls/ICRA2020Workshops.xlsx
+++ b/polls/ICRA2020Workshops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE068435-8A93-407B-884A-1E397D37C4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8421B8-7B8D-4D5F-8A13-FCF4D0D9EBA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1237,7 +1237,7 @@
   <dimension ref="A1:BJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>